<commit_message>
Class10 - Apache POI - Write to Excel
</commit_message>
<xml_diff>
--- a/testData/EmployeeList.xlsx
+++ b/testData/EmployeeList.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahnoza/IdeaProjects/SeleniumEx1/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahnoza/IdeaProjects/SeleniumNov2022/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683A55CC-4482-7E4E-BA84-F72DD3F6D1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29B4BEE-5D3E-844A-BD10-4BC7D07FB70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20200" yWindow="-17920" windowWidth="27300" windowHeight="14840" xr2:uid="{1D1C47EE-4C16-9B4F-8B18-1E6F1DCCC62A}"/>
+    <workbookView xWindow="-24040" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{1D1C47EE-4C16-9B4F-8B18-1E6F1DCCC62A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Firstname</t>
   </si>
@@ -133,6 +134,18 @@
   </si>
   <si>
     <t>Mike</t>
+  </si>
+  <si>
+    <t>Seniority Level</t>
+  </si>
+  <si>
+    <t>Mid-Level</t>
+  </si>
+  <si>
+    <t>Entry-Level</t>
+  </si>
+  <si>
+    <t>Senior-Level</t>
   </si>
 </sst>
 </file>
@@ -172,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -180,16 +193,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -505,95 +535,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4920DA02-DE11-354E-BC33-E43CCB871985}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="5">
         <v>105000</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="5">
         <v>90000</v>
       </c>
+      <c r="G3" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>120000</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -654,7 +697,7 @@
       <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E2" t="s">
@@ -679,4 +722,18 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I31" sqref="I31:I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>